<commit_message>
Add Firebase cost analysis and optimization reports - 60-day rolling window for assignments, attendance stats caching, incremental updates - Monthly cost: .11-.14 (~₹9-12) with 98% read reduction
</commit_message>
<xml_diff>
--- a/public/unom_template.xlsx
+++ b/public/unom_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanja\Documents\Edu Online\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3107CF7-9A81-4CCB-BD60-1BF9078EDE8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4A4E0F-8472-49F5-B103-EBCD83F2FDA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="150">
   <si>
     <t>VELTECH RANGA SANKU ARTS COLLEGE</t>
   </si>
@@ -489,9 +489,6 @@
   </si>
   <si>
     <t>PASS/FAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                  VELTECH RANGA SANKU ARTS COLLEGE</t>
   </si>
   <si>
     <t>[Department]  UNIVERSITY OF MADRAS EXAM RESULT ANALYSIS [month - year]                                       
@@ -1173,21 +1170,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1202,6 +1184,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1667,7 +1664,7 @@
   <dimension ref="A1:AI940"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="24" zoomScaleNormal="40" zoomScaleSheetLayoutView="10" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="A3" sqref="A3:AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1702,118 +1699,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="85.95" customHeight="1">
-      <c r="A1" s="86" t="s">
-        <v>149</v>
-      </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="86"/>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="86"/>
-      <c r="AC1" s="86"/>
-      <c r="AD1" s="86"/>
-      <c r="AE1" s="86"/>
-      <c r="AF1" s="86"/>
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81"/>
+      <c r="X1" s="81"/>
+      <c r="Y1" s="81"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="81"/>
+      <c r="AE1" s="81"/>
+      <c r="AF1" s="81"/>
       <c r="AG1" s="51"/>
       <c r="AH1" s="51"/>
       <c r="AI1" s="53"/>
     </row>
     <row r="2" spans="1:35" ht="155.4" customHeight="1">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="86"/>
-      <c r="S2" s="86"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="86"/>
-      <c r="V2" s="86"/>
-      <c r="W2" s="86"/>
-      <c r="X2" s="86"/>
-      <c r="Y2" s="86"/>
-      <c r="Z2" s="86"/>
-      <c r="AA2" s="86"/>
-      <c r="AB2" s="86"/>
-      <c r="AC2" s="86"/>
-      <c r="AD2" s="86"/>
-      <c r="AE2" s="86"/>
-      <c r="AF2" s="86"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
+      <c r="W2" s="81"/>
+      <c r="X2" s="81"/>
+      <c r="Y2" s="81"/>
+      <c r="Z2" s="81"/>
+      <c r="AA2" s="81"/>
+      <c r="AB2" s="81"/>
+      <c r="AC2" s="81"/>
+      <c r="AD2" s="81"/>
+      <c r="AE2" s="81"/>
+      <c r="AF2" s="81"/>
       <c r="AG2" s="51"/>
       <c r="AH2" s="51"/>
       <c r="AI2" s="53"/>
     </row>
     <row r="3" spans="1:35" ht="298.95" customHeight="1">
-      <c r="A3" s="87" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="87"/>
-      <c r="S3" s="87"/>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="87"/>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
-      <c r="Z3" s="87"/>
-      <c r="AA3" s="87"/>
-      <c r="AB3" s="87"/>
-      <c r="AC3" s="87"/>
-      <c r="AD3" s="87"/>
-      <c r="AE3" s="87"/>
-      <c r="AF3" s="87"/>
+      <c r="A3" s="82" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
+      <c r="AA3" s="82"/>
+      <c r="AB3" s="82"/>
+      <c r="AC3" s="82"/>
+      <c r="AD3" s="82"/>
+      <c r="AE3" s="82"/>
+      <c r="AF3" s="82"/>
       <c r="AG3" s="51"/>
       <c r="AH3" s="51"/>
       <c r="AI3" s="53"/>
@@ -1856,52 +1853,52 @@
       <c r="AI4" s="53"/>
     </row>
     <row r="5" spans="1:35" ht="194.1" customHeight="1">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="88"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="90"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="90"/>
-      <c r="T5" s="88"/>
-      <c r="U5" s="89"/>
-      <c r="V5" s="90"/>
-      <c r="W5" s="88"/>
-      <c r="X5" s="89"/>
-      <c r="Y5" s="90"/>
-      <c r="Z5" s="88"/>
-      <c r="AA5" s="89"/>
-      <c r="AB5" s="90"/>
-      <c r="AC5" s="82" t="s">
+      <c r="E5" s="83"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="83"/>
+      <c r="R5" s="84"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="84"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="84"/>
+      <c r="Y5" s="85"/>
+      <c r="Z5" s="83"/>
+      <c r="AA5" s="84"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="AD5" s="84" t="s">
+      <c r="AD5" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="AE5" s="84" t="s">
+      <c r="AE5" s="86" t="s">
         <v>147</v>
       </c>
-      <c r="AF5" s="84" t="s">
+      <c r="AF5" s="86" t="s">
         <v>148</v>
       </c>
       <c r="AG5" s="52"/>
@@ -1909,10 +1906,10 @@
       <c r="AI5" s="52"/>
     </row>
     <row r="6" spans="1:35" ht="303.89999999999998" customHeight="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="85"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
       <c r="E6" s="47"/>
       <c r="F6" s="47"/>
       <c r="G6" s="47"/>
@@ -1937,47 +1934,47 @@
       <c r="Z6" s="47"/>
       <c r="AA6" s="50"/>
       <c r="AB6" s="47"/>
-      <c r="AC6" s="83"/>
-      <c r="AD6" s="85"/>
-      <c r="AE6" s="85"/>
-      <c r="AF6" s="85"/>
+      <c r="AC6" s="90"/>
+      <c r="AD6" s="87"/>
+      <c r="AE6" s="87"/>
+      <c r="AF6" s="87"/>
       <c r="AG6" s="52"/>
       <c r="AH6" s="52"/>
       <c r="AI6" s="52"/>
     </row>
     <row r="7" spans="1:35" ht="81.75" customHeight="1">
-      <c r="A7" s="81"/>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="81"/>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
-      <c r="X7" s="81"/>
-      <c r="Y7" s="81"/>
-      <c r="Z7" s="81"/>
-      <c r="AA7" s="81"/>
-      <c r="AB7" s="81"/>
-      <c r="AC7" s="81"/>
-      <c r="AD7" s="81"/>
-      <c r="AE7" s="81"/>
-      <c r="AF7" s="81"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="88"/>
+      <c r="L7" s="88"/>
+      <c r="M7" s="88"/>
+      <c r="N7" s="88"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="88"/>
+      <c r="R7" s="88"/>
+      <c r="S7" s="88"/>
+      <c r="T7" s="88"/>
+      <c r="U7" s="88"/>
+      <c r="V7" s="88"/>
+      <c r="W7" s="88"/>
+      <c r="X7" s="88"/>
+      <c r="Y7" s="88"/>
+      <c r="Z7" s="88"/>
+      <c r="AA7" s="88"/>
+      <c r="AB7" s="88"/>
+      <c r="AC7" s="88"/>
+      <c r="AD7" s="88"/>
+      <c r="AE7" s="88"/>
+      <c r="AF7" s="88"/>
       <c r="AG7" s="53"/>
       <c r="AH7" s="53"/>
       <c r="AI7" s="53"/>
@@ -36432,6 +36429,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A7:AF7"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="AE5:AE6"/>
+    <mergeCell ref="AF5:AF6"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:AF2"/>
     <mergeCell ref="A3:AF3"/>
@@ -36447,11 +36449,6 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A7:AF7"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="AD5:AD6"/>
-    <mergeCell ref="AE5:AE6"/>
-    <mergeCell ref="AF5:AF6"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.23" bottom="0.74803149606299202" header="0.25" footer="0.31496062992126"/>

</xml_diff>